<commit_message>
incidentManagement.java IncidentReusables.java ChangeReusables.java ServiceNowUtils.java SuperTestNG.java WaitUtils.java HomePage.java IncidentPage.java Incident_Management_TestData.xlsx
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Incident_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Incident_Management_TestData.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Serial No.</t>
   </si>
@@ -117,70 +117,46 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>INC0020819</t>
-  </si>
-  <si>
-    <t>INC0020862</t>
+    <t>INC0020960</t>
+  </si>
+  <si>
+    <t>INC0021039</t>
+  </si>
+  <si>
+    <t>Sathyanarayanan V</t>
+  </si>
+  <si>
+    <t>Cause Code</t>
+  </si>
+  <si>
+    <t>Sub Cause Code</t>
+  </si>
+  <si>
+    <t>Mitigation and Solution Steps</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Change Failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitigation and Solution Steps for </t>
+  </si>
+  <si>
+    <t>testResolveIncidentTicket</t>
+  </si>
+  <si>
+    <t>Configuration Item</t>
+  </si>
+  <si>
+    <t>162LOAN-TPL-G</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>INC0020863</t>
-  </si>
-  <si>
-    <t>INC0020864</t>
-  </si>
-  <si>
-    <t>INC0020865</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>INC0020866</t>
-  </si>
-  <si>
-    <t>INC0020867</t>
-  </si>
-  <si>
-    <t>INC0020868</t>
-  </si>
-  <si>
-    <t>INC0020891</t>
-  </si>
-  <si>
-    <t>INC0020892</t>
-  </si>
-  <si>
-    <t>INC0020894</t>
-  </si>
-  <si>
-    <t>INC0020896</t>
-  </si>
-  <si>
-    <t>INC0020901</t>
-  </si>
-  <si>
-    <t>INC0020902</t>
-  </si>
-  <si>
-    <t>INC0020933</t>
-  </si>
-  <si>
-    <t>INC0020934</t>
-  </si>
-  <si>
-    <t>INC0020935</t>
-  </si>
-  <si>
-    <t>INC0020936</t>
-  </si>
-  <si>
-    <t>INC0020959</t>
-  </si>
-  <si>
-    <t>INC0020960</t>
+    <t>INC0021040</t>
   </si>
 </sst>
 </file>
@@ -275,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,6 +272,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" activeCellId="2" sqref="F2 F3 F5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -610,14 +589,15 @@
     <col min="11" max="11" bestFit="true" customWidth="true" width="16.5546875" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="20.5546875" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.88671875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="24">
+    <row r="1" spans="1:19" ht="24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,13 +637,22 @@
       <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="N1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
-    <row r="2" spans="1:18" ht="24">
+    <row r="2" spans="1:19" ht="24">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -671,7 +660,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" t="s">
@@ -699,11 +688,12 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="3"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
     </row>
-    <row r="3" spans="1:18" ht="24">
+    <row r="3" spans="1:19" ht="24">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -711,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
@@ -741,33 +731,51 @@
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="3"/>
+      <c r="P3" s="5"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="N4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -785,11 +793,12 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="3"/>
+      <c r="P5" s="5"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -807,9 +816,10 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="3"/>
+      <c r="P6" s="5"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Changes to incident modules and addition of Problem pages/ProblemPage.java, ProblemReusables.java, Problem_Management_TestData.xlsx, problemManagement.java
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Incident_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Incident_Management_TestData.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="113">
   <si>
     <t>Serial No.</t>
   </si>
@@ -202,6 +202,189 @@
   </si>
   <si>
     <t>INC0021227</t>
+  </si>
+  <si>
+    <t>INC0021272</t>
+  </si>
+  <si>
+    <t>INC0021279</t>
+  </si>
+  <si>
+    <t>INC0021280</t>
+  </si>
+  <si>
+    <t>INC0021281</t>
+  </si>
+  <si>
+    <t>INC0021321</t>
+  </si>
+  <si>
+    <t>INC0021324</t>
+  </si>
+  <si>
+    <t>INC0021325</t>
+  </si>
+  <si>
+    <t>INC0021326</t>
+  </si>
+  <si>
+    <t>INC0021464</t>
+  </si>
+  <si>
+    <t>INC0021465</t>
+  </si>
+  <si>
+    <t>INC0021466</t>
+  </si>
+  <si>
+    <t>INC0021467</t>
+  </si>
+  <si>
+    <t>INC0021468</t>
+  </si>
+  <si>
+    <t>INC0021469</t>
+  </si>
+  <si>
+    <t>INC0021470</t>
+  </si>
+  <si>
+    <t>INC0021471</t>
+  </si>
+  <si>
+    <t>INC0021472</t>
+  </si>
+  <si>
+    <t>INC0021473</t>
+  </si>
+  <si>
+    <t>INC0021474</t>
+  </si>
+  <si>
+    <t>INC0021475</t>
+  </si>
+  <si>
+    <t>INC0021476</t>
+  </si>
+  <si>
+    <t>INC0021477</t>
+  </si>
+  <si>
+    <t>INC0021478</t>
+  </si>
+  <si>
+    <t>INC0021479</t>
+  </si>
+  <si>
+    <t>INC0021480</t>
+  </si>
+  <si>
+    <t>INC0021481</t>
+  </si>
+  <si>
+    <t>INC0021482</t>
+  </si>
+  <si>
+    <t>INC0021483</t>
+  </si>
+  <si>
+    <t>INC0021484</t>
+  </si>
+  <si>
+    <t>INC0021485</t>
+  </si>
+  <si>
+    <t>INC0021486</t>
+  </si>
+  <si>
+    <t>INC0021487</t>
+  </si>
+  <si>
+    <t>INC0021488</t>
+  </si>
+  <si>
+    <t>INC0021489</t>
+  </si>
+  <si>
+    <t>INC0021490</t>
+  </si>
+  <si>
+    <t>INC0021491</t>
+  </si>
+  <si>
+    <t>INC0021492</t>
+  </si>
+  <si>
+    <t>INC0021493</t>
+  </si>
+  <si>
+    <t>INC0021494</t>
+  </si>
+  <si>
+    <t>INC0021495</t>
+  </si>
+  <si>
+    <t>INC0021605</t>
+  </si>
+  <si>
+    <t>INC0021606</t>
+  </si>
+  <si>
+    <t>INC0021608</t>
+  </si>
+  <si>
+    <t>INC0021609</t>
+  </si>
+  <si>
+    <t>INC0021610</t>
+  </si>
+  <si>
+    <t>INC0021611</t>
+  </si>
+  <si>
+    <t>INC0021612</t>
+  </si>
+  <si>
+    <t>INC0021613</t>
+  </si>
+  <si>
+    <t>INC0021614</t>
+  </si>
+  <si>
+    <t>INC0021746</t>
+  </si>
+  <si>
+    <t>INC0021747</t>
+  </si>
+  <si>
+    <t>INC0021748</t>
+  </si>
+  <si>
+    <t>INC0021752</t>
+  </si>
+  <si>
+    <t>INC0021753</t>
+  </si>
+  <si>
+    <t>INC0021754</t>
+  </si>
+  <si>
+    <t>INC0021755</t>
+  </si>
+  <si>
+    <t>INC0021757</t>
+  </si>
+  <si>
+    <t>INC0021758</t>
+  </si>
+  <si>
+    <t>INC0021759</t>
+  </si>
+  <si>
+    <t>INC0021760</t>
+  </si>
+  <si>
+    <t>INC0021761</t>
   </si>
 </sst>
 </file>
@@ -710,7 +893,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" t="s">
@@ -751,7 +934,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" t="s">
@@ -794,7 +977,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" t="s">
@@ -833,7 +1016,7 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" t="s">

</xml_diff>